<commit_message>
Updated proposal, ready for tomorrow
</commit_message>
<xml_diff>
--- a/Project_Proposal/Project_timeline_352.xlsx
+++ b/Project_Proposal/Project_timeline_352.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{F5063B6C-DBA1-456E-B3E2-6C04F6610922}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0624647E-FA43-4CAF-B83C-AC3943DEB7A0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Timeline" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>Activity</t>
   </si>
@@ -139,9 +139,6 @@
     <t>GUI Work for Gameplay</t>
   </si>
   <si>
-    <t>Additional Ideas(If time allows)</t>
-  </si>
-  <si>
     <t>Completed: Hunter</t>
   </si>
   <si>
@@ -149,6 +146,12 @@
   </si>
   <si>
     <t>Project Update</t>
+  </si>
+  <si>
+    <t>Not Completed</t>
+  </si>
+  <si>
+    <t>Combat/Leveling System</t>
   </si>
 </sst>
 </file>
@@ -376,14 +379,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -4569,7 +4572,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{343EE21F-E8BC-41C0-97DA-9A867CDDE9B6}</c15:txfldGUID>
+                      <c15:txfldGUID>{FECBF275-0635-4959-8EE3-A8E04D003AD5}</c15:txfldGUID>
                       <c15:f>calcs!$E$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4610,7 +4613,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{15FC7012-464D-46BA-B170-1B6909CC665A}</c15:txfldGUID>
+                      <c15:txfldGUID>{AB6D0302-C23C-4DB2-ADA5-868F5B81FD30}</c15:txfldGUID>
                       <c15:f>calcs!$F$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4651,7 +4654,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3F69102E-5496-4C10-AC79-599B5204049D}</c15:txfldGUID>
+                      <c15:txfldGUID>{753C0980-5248-4A27-BD96-CA578B015E0C}</c15:txfldGUID>
                       <c15:f>calcs!$G$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4692,7 +4695,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{42956297-4F1D-4326-B9AF-4F00F8674F45}</c15:txfldGUID>
+                      <c15:txfldGUID>{BAA34394-1863-4E49-8FA7-089BF2821A36}</c15:txfldGUID>
                       <c15:f>calcs!$H$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4733,7 +4736,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0573868D-8DD5-4A6F-837D-C2553D00DF21}</c15:txfldGUID>
+                      <c15:txfldGUID>{53D1FE3D-E7EB-47A4-9322-AABEE7E52110}</c15:txfldGUID>
                       <c15:f>calcs!$I$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4774,7 +4777,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{BFA61052-1559-4114-ACBD-A17345085941}</c15:txfldGUID>
+                      <c15:txfldGUID>{5FF616DD-E2E2-4AB6-8784-5E09D69F9543}</c15:txfldGUID>
                       <c15:f>calcs!$J$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4815,7 +4818,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3D9C27AD-9C28-4735-A26A-BA502052E1A1}</c15:txfldGUID>
+                      <c15:txfldGUID>{6A864164-7792-45AE-A58B-B970E6F1ACB3}</c15:txfldGUID>
                       <c15:f>calcs!$K$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4856,7 +4859,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7CD90C6F-D783-48BB-840A-706F2B827CB0}</c15:txfldGUID>
+                      <c15:txfldGUID>{BA7A39FA-7258-416E-8C95-7A896E796EE4}</c15:txfldGUID>
                       <c15:f>calcs!$L$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4897,7 +4900,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A975F67A-D4F5-4EDE-BC5C-CE327738B5F6}</c15:txfldGUID>
+                      <c15:txfldGUID>{C1B7F649-9BB2-4E03-9053-F4D92AB7C630}</c15:txfldGUID>
                       <c15:f>calcs!$M$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4938,7 +4941,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D9216560-1264-473D-A5F3-1F149F428341}</c15:txfldGUID>
+                      <c15:txfldGUID>{8490428F-74E2-44D2-A644-CEFC7FD8DE8E}</c15:txfldGUID>
                       <c15:f>calcs!$N$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4979,7 +4982,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{82954CE9-89CF-4373-939E-CC4B85251545}</c15:txfldGUID>
+                      <c15:txfldGUID>{30B5BE9E-104D-45AF-A559-9125DC008DD9}</c15:txfldGUID>
                       <c15:f>calcs!$O$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5020,7 +5023,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E0E644A2-A348-4C9C-BC3D-868BC5901CFC}</c15:txfldGUID>
+                      <c15:txfldGUID>{DD387200-581C-4679-A50E-53448A14FB24}</c15:txfldGUID>
                       <c15:f>calcs!$P$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5061,7 +5064,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8967893E-7761-4312-AE25-3CF615796174}</c15:txfldGUID>
+                      <c15:txfldGUID>{7EA2F090-7874-47EC-96D0-154D20132DA4}</c15:txfldGUID>
                       <c15:f>calcs!$Q$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5102,7 +5105,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4CF427D4-075C-41A3-B404-2D6AE1B878E5}</c15:txfldGUID>
+                      <c15:txfldGUID>{D206F15F-B553-43DA-A9DA-6ADAA167F438}</c15:txfldGUID>
                       <c15:f>calcs!$R$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5143,7 +5146,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7AA65F18-A6A2-4A03-A536-9ECA6561CB40}</c15:txfldGUID>
+                      <c15:txfldGUID>{8CDBCBDF-06D4-4530-925D-C5606B85C81F}</c15:txfldGUID>
                       <c15:f>calcs!$S$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5184,7 +5187,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{2B110E85-BCD8-4A9E-8387-86DC4C056F42}</c15:txfldGUID>
+                      <c15:txfldGUID>{CE1D7751-304B-4711-AD79-9391B61CFC97}</c15:txfldGUID>
                       <c15:f>calcs!$T$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5225,7 +5228,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{253F6488-4BF2-417C-91F4-30884154BF69}</c15:txfldGUID>
+                      <c15:txfldGUID>{98AE7B59-20F4-4374-9E15-C34B0D6F348D}</c15:txfldGUID>
                       <c15:f>calcs!$U$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5266,7 +5269,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{584DC2FA-004E-4B4C-92FA-EA2989F80F91}</c15:txfldGUID>
+                      <c15:txfldGUID>{27676B1F-E514-435D-A57F-74E54BAD8380}</c15:txfldGUID>
                       <c15:f>calcs!$V$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5307,7 +5310,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A34A451F-DF7B-4DDF-8594-68E266BEB0FA}</c15:txfldGUID>
+                      <c15:txfldGUID>{D9D1B390-30DB-4FBB-990F-B1F19E6E6AC7}</c15:txfldGUID>
                       <c15:f>calcs!$W$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5348,7 +5351,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{67AD41C3-8836-421B-9D7D-D7560371A135}</c15:txfldGUID>
+                      <c15:txfldGUID>{F70F91F7-FDBE-419C-8172-CC31CFC4F525}</c15:txfldGUID>
                       <c15:f>calcs!$X$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5389,7 +5392,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5C37C8F5-3ACD-4FD0-8948-4334A91C4751}</c15:txfldGUID>
+                      <c15:txfldGUID>{E93EDF26-091B-4D18-8751-FE5337523C69}</c15:txfldGUID>
                       <c15:f>calcs!$Y$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5430,7 +5433,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E081194C-030C-4F5E-AD5B-62D624A87E25}</c15:txfldGUID>
+                      <c15:txfldGUID>{44DE2064-8F6E-4A0D-80C1-8769FAEF9629}</c15:txfldGUID>
                       <c15:f>calcs!$Z$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5471,7 +5474,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{FFB9C84F-385F-44D1-8837-5E0263C52987}</c15:txfldGUID>
+                      <c15:txfldGUID>{D547AA9E-FF6F-472F-ABAF-8955FB98B3A0}</c15:txfldGUID>
                       <c15:f>calcs!$AA$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5512,7 +5515,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{F773A87E-6290-45CE-B1B7-A5951B8DB48D}</c15:txfldGUID>
+                      <c15:txfldGUID>{E97C0ECD-D82C-444D-B9AF-1610A65C7C3B}</c15:txfldGUID>
                       <c15:f>calcs!$AB$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5553,7 +5556,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8CAF1ECA-FAB8-4CB0-9F41-C63721C3ACB1}</c15:txfldGUID>
+                      <c15:txfldGUID>{0EB4F08E-B6A5-4935-B639-04744E600B87}</c15:txfldGUID>
                       <c15:f>calcs!$AC$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5594,7 +5597,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E2F9F11F-B92A-4441-AB91-0B08E786E764}</c15:txfldGUID>
+                      <c15:txfldGUID>{9746D9C5-2AF0-4AAC-878E-F1A0CA41F666}</c15:txfldGUID>
                       <c15:f>calcs!$AD$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5635,7 +5638,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D35780DD-B91C-4A54-87A3-037EE8B3B765}</c15:txfldGUID>
+                      <c15:txfldGUID>{763D5189-220F-4EE0-A06A-3F35CDA102C9}</c15:txfldGUID>
                       <c15:f>calcs!$AE$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5676,7 +5679,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0B4A78A4-1A1E-4E74-9E1F-B86122E45505}</c15:txfldGUID>
+                      <c15:txfldGUID>{77EE5407-5027-4EDE-88F4-BAEE066D7B73}</c15:txfldGUID>
                       <c15:f>calcs!$AF$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5717,7 +5720,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{14519BDE-2637-4475-8FA7-73B1B4EA37FF}</c15:txfldGUID>
+                      <c15:txfldGUID>{A91620A1-F9BF-4702-8F07-06EB7813832E}</c15:txfldGUID>
                       <c15:f>calcs!$AG$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5758,7 +5761,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4A34D628-3282-45B4-8581-FE107B97710D}</c15:txfldGUID>
+                      <c15:txfldGUID>{36390404-28EB-4FBE-AE62-502A8189F4FB}</c15:txfldGUID>
                       <c15:f>calcs!$AH$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5951,7 +5954,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A7991C22-5339-4777-B698-D6BCB4219B9E}</c15:txfldGUID>
+                      <c15:txfldGUID>{06EF337E-44B1-482D-9377-A5B413CB62F1}</c15:txfldGUID>
                       <c15:f>calcs!$E$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5992,7 +5995,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{176C18AB-A490-487B-9F93-8AB4A93B215A}</c15:txfldGUID>
+                      <c15:txfldGUID>{BC029AEF-69E6-46CA-81D3-73678B0D1C5D}</c15:txfldGUID>
                       <c15:f>calcs!$F$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6033,7 +6036,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E4FECFC0-7291-4911-B52A-582D28AE1E0C}</c15:txfldGUID>
+                      <c15:txfldGUID>{ECC110A8-2289-446E-89C2-832E45B820F4}</c15:txfldGUID>
                       <c15:f>calcs!$G$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6074,7 +6077,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{77739588-1B24-4A66-8DD8-DDF4709CCD39}</c15:txfldGUID>
+                      <c15:txfldGUID>{7908983E-59E2-4C92-AC44-D9D47B8CAEE5}</c15:txfldGUID>
                       <c15:f>calcs!$H$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6115,7 +6118,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{DF025A74-4E81-496E-B37A-B65D88A94CB5}</c15:txfldGUID>
+                      <c15:txfldGUID>{06DA021C-786D-4CFA-B3F3-68110C8A5953}</c15:txfldGUID>
                       <c15:f>calcs!$I$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6156,7 +6159,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{DCA740C5-DA71-4806-89F1-9840BA30294C}</c15:txfldGUID>
+                      <c15:txfldGUID>{B9167896-9A0A-449A-912E-E8C0705FF850}</c15:txfldGUID>
                       <c15:f>calcs!$J$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6197,7 +6200,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8BD641A2-1A48-47D2-8830-61897D8B0722}</c15:txfldGUID>
+                      <c15:txfldGUID>{D66AF605-A7CE-4370-B0E6-13DE4A997F98}</c15:txfldGUID>
                       <c15:f>calcs!$K$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6238,7 +6241,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5639397B-3390-4550-A74F-79EA1B046D73}</c15:txfldGUID>
+                      <c15:txfldGUID>{FF7177CC-22EF-4207-B31F-464E29B757C1}</c15:txfldGUID>
                       <c15:f>calcs!$L$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6279,7 +6282,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{41387C92-DE37-44CE-BEAC-B224FB4A3CCF}</c15:txfldGUID>
+                      <c15:txfldGUID>{3C1484B7-F99C-44CB-9E7A-B55D8C514CA0}</c15:txfldGUID>
                       <c15:f>calcs!$M$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6320,7 +6323,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3B5F7BAB-174E-46A2-B2A1-4F207FCF6B17}</c15:txfldGUID>
+                      <c15:txfldGUID>{CE1A255D-12D6-4613-8490-8EDD727D0AEB}</c15:txfldGUID>
                       <c15:f>calcs!$N$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6361,7 +6364,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{463E6116-FEEB-43E0-87DE-4D53481E03C1}</c15:txfldGUID>
+                      <c15:txfldGUID>{E197CB41-4224-4077-AB39-59866F828AC0}</c15:txfldGUID>
                       <c15:f>calcs!$O$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6402,7 +6405,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{922DA5A0-AFB9-4E43-8A9C-41CC422294E8}</c15:txfldGUID>
+                      <c15:txfldGUID>{5F0BF020-127F-40B7-8EE4-F3F1A307E48C}</c15:txfldGUID>
                       <c15:f>calcs!$P$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6443,7 +6446,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A870AE15-000E-40E7-87E2-3F286CF7A400}</c15:txfldGUID>
+                      <c15:txfldGUID>{2C6398D2-8380-403E-B414-9697A4C4B3BB}</c15:txfldGUID>
                       <c15:f>calcs!$Q$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6484,7 +6487,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{72AFCFCB-017F-4E5B-BC53-716F71426364}</c15:txfldGUID>
+                      <c15:txfldGUID>{5D2B9DFC-96EE-47D2-BD38-444458555567}</c15:txfldGUID>
                       <c15:f>calcs!$R$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6525,7 +6528,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{F352F334-8DE2-4758-8134-9883AF16CEA2}</c15:txfldGUID>
+                      <c15:txfldGUID>{0F8B3916-C3C2-4F7C-8CA7-6CC012E72DC2}</c15:txfldGUID>
                       <c15:f>calcs!$S$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6566,7 +6569,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{208D0400-58C8-4406-97EE-A78626E98213}</c15:txfldGUID>
+                      <c15:txfldGUID>{5B64ED67-5F21-4278-AF7D-8E6EEEE3B1D8}</c15:txfldGUID>
                       <c15:f>calcs!$T$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6607,7 +6610,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5160F406-2704-40AC-BB1D-481721E9CA0E}</c15:txfldGUID>
+                      <c15:txfldGUID>{6042171F-F494-4AE0-84FF-201F6D6D5DB7}</c15:txfldGUID>
                       <c15:f>calcs!$U$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6648,7 +6651,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{F2FF2350-C333-414F-A1E6-7A04CF56EF8A}</c15:txfldGUID>
+                      <c15:txfldGUID>{C03256AC-BA83-4C8E-BAC8-DCFA9198873C}</c15:txfldGUID>
                       <c15:f>calcs!$V$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6689,7 +6692,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{88611894-D76C-4647-9617-ABA60AFB4BEA}</c15:txfldGUID>
+                      <c15:txfldGUID>{04D92674-82A7-4408-BFC1-68739034B17A}</c15:txfldGUID>
                       <c15:f>calcs!$W$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6730,7 +6733,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{47657DF3-FC9B-40D2-BB35-A3E28A96D17D}</c15:txfldGUID>
+                      <c15:txfldGUID>{D1230F48-6512-4F89-B8E9-28C5A13CA4F9}</c15:txfldGUID>
                       <c15:f>calcs!$X$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6771,7 +6774,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{52B68A95-0F7D-4E92-AC23-C253495D1B0A}</c15:txfldGUID>
+                      <c15:txfldGUID>{4E12AF0F-0D0B-47BB-9CDB-6A1C00D90FDE}</c15:txfldGUID>
                       <c15:f>calcs!$Y$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6812,7 +6815,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{EC35CF58-29A0-4B70-8996-746588ED1A67}</c15:txfldGUID>
+                      <c15:txfldGUID>{2D67A013-77E9-43E9-90D1-19EF6A389879}</c15:txfldGUID>
                       <c15:f>calcs!$Z$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6853,7 +6856,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3D63415A-2314-4DCB-98DB-CC33BEF0D329}</c15:txfldGUID>
+                      <c15:txfldGUID>{B40432EE-35D1-4CDA-8CB6-CAAD3022A67D}</c15:txfldGUID>
                       <c15:f>calcs!$AA$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6894,7 +6897,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A6589455-1124-40A3-8051-DB318BBA9263}</c15:txfldGUID>
+                      <c15:txfldGUID>{EB840C98-F01C-4969-A553-21B1526E6092}</c15:txfldGUID>
                       <c15:f>calcs!$AB$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6935,7 +6938,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{2C5A96F3-1ED3-48D6-9E7F-F63EFB495E0A}</c15:txfldGUID>
+                      <c15:txfldGUID>{7DEBE99F-D53E-4998-9E38-0015FF2529B4}</c15:txfldGUID>
                       <c15:f>calcs!$AC$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6976,7 +6979,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{CE072F2A-C688-4688-87E0-20AFBDA2A93C}</c15:txfldGUID>
+                      <c15:txfldGUID>{2D1ECED0-68E7-4F75-AAC1-77F4861D917D}</c15:txfldGUID>
                       <c15:f>calcs!$AD$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -7017,7 +7020,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4DE14F4B-7D65-4FC1-975A-BDD056234996}</c15:txfldGUID>
+                      <c15:txfldGUID>{E683EA6D-20E0-4A85-B1EC-0B8366D760B2}</c15:txfldGUID>
                       <c15:f>calcs!$AE$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -7058,7 +7061,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D619C517-DAFC-43CD-B0E2-249F7E14DBBD}</c15:txfldGUID>
+                      <c15:txfldGUID>{5DD9D42F-8F20-4BAD-A57C-D04CE5E5A26D}</c15:txfldGUID>
                       <c15:f>calcs!$AF$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -7099,7 +7102,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4B1812C2-D419-40AD-9C59-79DDFD2B87D5}</c15:txfldGUID>
+                      <c15:txfldGUID>{A14925E9-CEDC-4F5F-B21E-91B924257B04}</c15:txfldGUID>
                       <c15:f>calcs!$AG$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -7140,7 +7143,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5394315F-FA09-4AB6-98C6-F23522E72F64}</c15:txfldGUID>
+                      <c15:txfldGUID>{4209D686-BB72-41AF-A8D6-34EF921251AD}</c15:txfldGUID>
                       <c15:f>calcs!$AH$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -7719,8 +7722,8 @@
         <a:xfrm>
           <a:off x="325877" y="4038600"/>
           <a:ext cx="8988869" cy="228436"/>
-          <a:chOff x="306828" y="4108026"/>
-          <a:chExt cx="8729080" cy="223568"/>
+          <a:chOff x="306828" y="4108028"/>
+          <a:chExt cx="8729080" cy="223566"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
@@ -7794,7 +7797,7 @@
             </xdr:nvSpPr>
             <xdr:spPr bwMode="auto">
               <a:xfrm>
-                <a:off x="306828" y="4108026"/>
+                <a:off x="306828" y="4108028"/>
                 <a:ext cx="8729080" cy="163196"/>
               </a:xfrm>
               <a:prstGeom prst="rect">
@@ -8078,8 +8081,8 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8096,22 +8099,22 @@
     <row r="1" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" ht="315.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:7" s="7" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="8" t="s">
@@ -8251,7 +8254,7 @@
         <v>43760</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -8271,7 +8274,7 @@
         <v>43778</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -8291,7 +8294,7 @@
         <v>43772</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -8299,14 +8302,17 @@
         <f>ROW(B13)-calcs!$D$5</f>
         <v>-2</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>37</v>
+      <c r="C13" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="D13" s="1">
         <v>43786</v>
       </c>
       <c r="E13" s="1">
         <v>43786</v>
+      </c>
+      <c r="F13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -8314,7 +8320,7 @@
         <f>ROW(B14)-calcs!$D$5</f>
         <v>-1</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="11" t="s">
         <v>31</v>
       </c>
       <c r="D14" s="5">
@@ -8324,6 +8330,9 @@
       <c r="E14" s="5">
         <f>Activities[[#This Row],[START]]+7</f>
         <v>43789</v>
+      </c>
+      <c r="F14" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -8331,7 +8340,7 @@
         <f>ROW(B15)-calcs!$D$5</f>
         <v>0</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="11" t="s">
         <v>32</v>
       </c>
       <c r="D15" s="5">
@@ -8341,6 +8350,9 @@
       <c r="E15" s="5">
         <f>Activities[[#This Row],[START]]+6</f>
         <v>43793</v>
+      </c>
+      <c r="F15" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -8348,7 +8360,7 @@
         <f>ROW(B16)-calcs!$D$5</f>
         <v>1</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>33</v>
       </c>
       <c r="D16" s="5">
@@ -8358,14 +8370,17 @@
         <f>Activities[[#This Row],[START]]+8</f>
         <v>43797</v>
       </c>
+      <c r="F16" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="17" spans="2:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>ROW(B17)-calcs!$D$5</f>
         <v>2</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>34</v>
+      <c r="C17" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="D17" s="5">
         <f>D16+2</f>
@@ -8374,25 +8389,28 @@
       <c r="E17" s="5">
         <v>43804</v>
       </c>
+      <c r="F17" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="18" spans="2:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18">
         <f>ROW(B18)-calcs!$D$5</f>
         <v>3</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="11" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="1">
         <v>43804</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19">
         <f>ROW(B19)-calcs!$D$5</f>
         <v>4</v>
       </c>
-      <c r="C19" s="13"/>
+      <c r="C19" s="11"/>
       <c r="D19" s="1"/>
     </row>
   </sheetData>
@@ -8481,7 +8499,7 @@
       </c>
       <c r="D3" s="1">
         <f ca="1">TODAY()</f>
-        <v>43785</v>
+        <v>43801</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -12899,23 +12917,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9677210f24a1be23c92c90fd886aa0aa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="60e05723c5c1908df1a1a4ebf11d344e" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -13126,25 +13127,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED11D93F-21D3-4821-9768-A0F99C41A8EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{983CAFE3-5C64-4732-BD1D-A9D00643597D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5BB6EA-B4A9-4FD0-A581-32FE787E0D00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13161,4 +13161,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{983CAFE3-5C64-4732-BD1D-A9D00643597D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED11D93F-21D3-4821-9768-A0F99C41A8EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Tweaked some stuff for the final demo
</commit_message>
<xml_diff>
--- a/Project_Proposal/Project_timeline_352.xlsx
+++ b/Project_Proposal/Project_timeline_352.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{F5063B6C-DBA1-456E-B3E2-6C04F6610922}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0624647E-FA43-4CAF-B83C-AC3943DEB7A0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Timeline" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>Activity</t>
   </si>
@@ -139,9 +139,6 @@
     <t>GUI Work for Gameplay</t>
   </si>
   <si>
-    <t>Additional Ideas(If time allows)</t>
-  </si>
-  <si>
     <t>Completed: Hunter</t>
   </si>
   <si>
@@ -149,6 +146,12 @@
   </si>
   <si>
     <t>Project Update</t>
+  </si>
+  <si>
+    <t>Not Completed</t>
+  </si>
+  <si>
+    <t>Combat/Leveling System</t>
   </si>
 </sst>
 </file>
@@ -376,14 +379,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -4569,7 +4572,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{343EE21F-E8BC-41C0-97DA-9A867CDDE9B6}</c15:txfldGUID>
+                      <c15:txfldGUID>{FECBF275-0635-4959-8EE3-A8E04D003AD5}</c15:txfldGUID>
                       <c15:f>calcs!$E$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4610,7 +4613,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{15FC7012-464D-46BA-B170-1B6909CC665A}</c15:txfldGUID>
+                      <c15:txfldGUID>{AB6D0302-C23C-4DB2-ADA5-868F5B81FD30}</c15:txfldGUID>
                       <c15:f>calcs!$F$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4651,7 +4654,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3F69102E-5496-4C10-AC79-599B5204049D}</c15:txfldGUID>
+                      <c15:txfldGUID>{753C0980-5248-4A27-BD96-CA578B015E0C}</c15:txfldGUID>
                       <c15:f>calcs!$G$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4692,7 +4695,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{42956297-4F1D-4326-B9AF-4F00F8674F45}</c15:txfldGUID>
+                      <c15:txfldGUID>{BAA34394-1863-4E49-8FA7-089BF2821A36}</c15:txfldGUID>
                       <c15:f>calcs!$H$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4733,7 +4736,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0573868D-8DD5-4A6F-837D-C2553D00DF21}</c15:txfldGUID>
+                      <c15:txfldGUID>{53D1FE3D-E7EB-47A4-9322-AABEE7E52110}</c15:txfldGUID>
                       <c15:f>calcs!$I$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4774,7 +4777,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{BFA61052-1559-4114-ACBD-A17345085941}</c15:txfldGUID>
+                      <c15:txfldGUID>{5FF616DD-E2E2-4AB6-8784-5E09D69F9543}</c15:txfldGUID>
                       <c15:f>calcs!$J$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4815,7 +4818,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3D9C27AD-9C28-4735-A26A-BA502052E1A1}</c15:txfldGUID>
+                      <c15:txfldGUID>{6A864164-7792-45AE-A58B-B970E6F1ACB3}</c15:txfldGUID>
                       <c15:f>calcs!$K$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4856,7 +4859,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7CD90C6F-D783-48BB-840A-706F2B827CB0}</c15:txfldGUID>
+                      <c15:txfldGUID>{BA7A39FA-7258-416E-8C95-7A896E796EE4}</c15:txfldGUID>
                       <c15:f>calcs!$L$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4897,7 +4900,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A975F67A-D4F5-4EDE-BC5C-CE327738B5F6}</c15:txfldGUID>
+                      <c15:txfldGUID>{C1B7F649-9BB2-4E03-9053-F4D92AB7C630}</c15:txfldGUID>
                       <c15:f>calcs!$M$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4938,7 +4941,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D9216560-1264-473D-A5F3-1F149F428341}</c15:txfldGUID>
+                      <c15:txfldGUID>{8490428F-74E2-44D2-A644-CEFC7FD8DE8E}</c15:txfldGUID>
                       <c15:f>calcs!$N$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -4979,7 +4982,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{82954CE9-89CF-4373-939E-CC4B85251545}</c15:txfldGUID>
+                      <c15:txfldGUID>{30B5BE9E-104D-45AF-A559-9125DC008DD9}</c15:txfldGUID>
                       <c15:f>calcs!$O$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5020,7 +5023,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E0E644A2-A348-4C9C-BC3D-868BC5901CFC}</c15:txfldGUID>
+                      <c15:txfldGUID>{DD387200-581C-4679-A50E-53448A14FB24}</c15:txfldGUID>
                       <c15:f>calcs!$P$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5061,7 +5064,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8967893E-7761-4312-AE25-3CF615796174}</c15:txfldGUID>
+                      <c15:txfldGUID>{7EA2F090-7874-47EC-96D0-154D20132DA4}</c15:txfldGUID>
                       <c15:f>calcs!$Q$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5102,7 +5105,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4CF427D4-075C-41A3-B404-2D6AE1B878E5}</c15:txfldGUID>
+                      <c15:txfldGUID>{D206F15F-B553-43DA-A9DA-6ADAA167F438}</c15:txfldGUID>
                       <c15:f>calcs!$R$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5143,7 +5146,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{7AA65F18-A6A2-4A03-A536-9ECA6561CB40}</c15:txfldGUID>
+                      <c15:txfldGUID>{8CDBCBDF-06D4-4530-925D-C5606B85C81F}</c15:txfldGUID>
                       <c15:f>calcs!$S$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5184,7 +5187,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{2B110E85-BCD8-4A9E-8387-86DC4C056F42}</c15:txfldGUID>
+                      <c15:txfldGUID>{CE1D7751-304B-4711-AD79-9391B61CFC97}</c15:txfldGUID>
                       <c15:f>calcs!$T$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5225,7 +5228,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{253F6488-4BF2-417C-91F4-30884154BF69}</c15:txfldGUID>
+                      <c15:txfldGUID>{98AE7B59-20F4-4374-9E15-C34B0D6F348D}</c15:txfldGUID>
                       <c15:f>calcs!$U$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5266,7 +5269,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{584DC2FA-004E-4B4C-92FA-EA2989F80F91}</c15:txfldGUID>
+                      <c15:txfldGUID>{27676B1F-E514-435D-A57F-74E54BAD8380}</c15:txfldGUID>
                       <c15:f>calcs!$V$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5307,7 +5310,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A34A451F-DF7B-4DDF-8594-68E266BEB0FA}</c15:txfldGUID>
+                      <c15:txfldGUID>{D9D1B390-30DB-4FBB-990F-B1F19E6E6AC7}</c15:txfldGUID>
                       <c15:f>calcs!$W$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5348,7 +5351,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{67AD41C3-8836-421B-9D7D-D7560371A135}</c15:txfldGUID>
+                      <c15:txfldGUID>{F70F91F7-FDBE-419C-8172-CC31CFC4F525}</c15:txfldGUID>
                       <c15:f>calcs!$X$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5389,7 +5392,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5C37C8F5-3ACD-4FD0-8948-4334A91C4751}</c15:txfldGUID>
+                      <c15:txfldGUID>{E93EDF26-091B-4D18-8751-FE5337523C69}</c15:txfldGUID>
                       <c15:f>calcs!$Y$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5430,7 +5433,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E081194C-030C-4F5E-AD5B-62D624A87E25}</c15:txfldGUID>
+                      <c15:txfldGUID>{44DE2064-8F6E-4A0D-80C1-8769FAEF9629}</c15:txfldGUID>
                       <c15:f>calcs!$Z$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5471,7 +5474,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{FFB9C84F-385F-44D1-8837-5E0263C52987}</c15:txfldGUID>
+                      <c15:txfldGUID>{D547AA9E-FF6F-472F-ABAF-8955FB98B3A0}</c15:txfldGUID>
                       <c15:f>calcs!$AA$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5512,7 +5515,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{F773A87E-6290-45CE-B1B7-A5951B8DB48D}</c15:txfldGUID>
+                      <c15:txfldGUID>{E97C0ECD-D82C-444D-B9AF-1610A65C7C3B}</c15:txfldGUID>
                       <c15:f>calcs!$AB$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5553,7 +5556,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8CAF1ECA-FAB8-4CB0-9F41-C63721C3ACB1}</c15:txfldGUID>
+                      <c15:txfldGUID>{0EB4F08E-B6A5-4935-B639-04744E600B87}</c15:txfldGUID>
                       <c15:f>calcs!$AC$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5594,7 +5597,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E2F9F11F-B92A-4441-AB91-0B08E786E764}</c15:txfldGUID>
+                      <c15:txfldGUID>{9746D9C5-2AF0-4AAC-878E-F1A0CA41F666}</c15:txfldGUID>
                       <c15:f>calcs!$AD$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5635,7 +5638,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D35780DD-B91C-4A54-87A3-037EE8B3B765}</c15:txfldGUID>
+                      <c15:txfldGUID>{763D5189-220F-4EE0-A06A-3F35CDA102C9}</c15:txfldGUID>
                       <c15:f>calcs!$AE$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5676,7 +5679,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0B4A78A4-1A1E-4E74-9E1F-B86122E45505}</c15:txfldGUID>
+                      <c15:txfldGUID>{77EE5407-5027-4EDE-88F4-BAEE066D7B73}</c15:txfldGUID>
                       <c15:f>calcs!$AF$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5717,7 +5720,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{14519BDE-2637-4475-8FA7-73B1B4EA37FF}</c15:txfldGUID>
+                      <c15:txfldGUID>{A91620A1-F9BF-4702-8F07-06EB7813832E}</c15:txfldGUID>
                       <c15:f>calcs!$AG$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5758,7 +5761,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4A34D628-3282-45B4-8581-FE107B97710D}</c15:txfldGUID>
+                      <c15:txfldGUID>{36390404-28EB-4FBE-AE62-502A8189F4FB}</c15:txfldGUID>
                       <c15:f>calcs!$AH$72</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5951,7 +5954,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A7991C22-5339-4777-B698-D6BCB4219B9E}</c15:txfldGUID>
+                      <c15:txfldGUID>{06EF337E-44B1-482D-9377-A5B413CB62F1}</c15:txfldGUID>
                       <c15:f>calcs!$E$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -5992,7 +5995,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{176C18AB-A490-487B-9F93-8AB4A93B215A}</c15:txfldGUID>
+                      <c15:txfldGUID>{BC029AEF-69E6-46CA-81D3-73678B0D1C5D}</c15:txfldGUID>
                       <c15:f>calcs!$F$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6033,7 +6036,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{E4FECFC0-7291-4911-B52A-582D28AE1E0C}</c15:txfldGUID>
+                      <c15:txfldGUID>{ECC110A8-2289-446E-89C2-832E45B820F4}</c15:txfldGUID>
                       <c15:f>calcs!$G$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6074,7 +6077,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{77739588-1B24-4A66-8DD8-DDF4709CCD39}</c15:txfldGUID>
+                      <c15:txfldGUID>{7908983E-59E2-4C92-AC44-D9D47B8CAEE5}</c15:txfldGUID>
                       <c15:f>calcs!$H$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6115,7 +6118,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{DF025A74-4E81-496E-B37A-B65D88A94CB5}</c15:txfldGUID>
+                      <c15:txfldGUID>{06DA021C-786D-4CFA-B3F3-68110C8A5953}</c15:txfldGUID>
                       <c15:f>calcs!$I$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6156,7 +6159,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{DCA740C5-DA71-4806-89F1-9840BA30294C}</c15:txfldGUID>
+                      <c15:txfldGUID>{B9167896-9A0A-449A-912E-E8C0705FF850}</c15:txfldGUID>
                       <c15:f>calcs!$J$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6197,7 +6200,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{8BD641A2-1A48-47D2-8830-61897D8B0722}</c15:txfldGUID>
+                      <c15:txfldGUID>{D66AF605-A7CE-4370-B0E6-13DE4A997F98}</c15:txfldGUID>
                       <c15:f>calcs!$K$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6238,7 +6241,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5639397B-3390-4550-A74F-79EA1B046D73}</c15:txfldGUID>
+                      <c15:txfldGUID>{FF7177CC-22EF-4207-B31F-464E29B757C1}</c15:txfldGUID>
                       <c15:f>calcs!$L$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6279,7 +6282,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{41387C92-DE37-44CE-BEAC-B224FB4A3CCF}</c15:txfldGUID>
+                      <c15:txfldGUID>{3C1484B7-F99C-44CB-9E7A-B55D8C514CA0}</c15:txfldGUID>
                       <c15:f>calcs!$M$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6320,7 +6323,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3B5F7BAB-174E-46A2-B2A1-4F207FCF6B17}</c15:txfldGUID>
+                      <c15:txfldGUID>{CE1A255D-12D6-4613-8490-8EDD727D0AEB}</c15:txfldGUID>
                       <c15:f>calcs!$N$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6361,7 +6364,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{463E6116-FEEB-43E0-87DE-4D53481E03C1}</c15:txfldGUID>
+                      <c15:txfldGUID>{E197CB41-4224-4077-AB39-59866F828AC0}</c15:txfldGUID>
                       <c15:f>calcs!$O$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6402,7 +6405,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{922DA5A0-AFB9-4E43-8A9C-41CC422294E8}</c15:txfldGUID>
+                      <c15:txfldGUID>{5F0BF020-127F-40B7-8EE4-F3F1A307E48C}</c15:txfldGUID>
                       <c15:f>calcs!$P$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6443,7 +6446,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A870AE15-000E-40E7-87E2-3F286CF7A400}</c15:txfldGUID>
+                      <c15:txfldGUID>{2C6398D2-8380-403E-B414-9697A4C4B3BB}</c15:txfldGUID>
                       <c15:f>calcs!$Q$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6484,7 +6487,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{72AFCFCB-017F-4E5B-BC53-716F71426364}</c15:txfldGUID>
+                      <c15:txfldGUID>{5D2B9DFC-96EE-47D2-BD38-444458555567}</c15:txfldGUID>
                       <c15:f>calcs!$R$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6525,7 +6528,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{F352F334-8DE2-4758-8134-9883AF16CEA2}</c15:txfldGUID>
+                      <c15:txfldGUID>{0F8B3916-C3C2-4F7C-8CA7-6CC012E72DC2}</c15:txfldGUID>
                       <c15:f>calcs!$S$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6566,7 +6569,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{208D0400-58C8-4406-97EE-A78626E98213}</c15:txfldGUID>
+                      <c15:txfldGUID>{5B64ED67-5F21-4278-AF7D-8E6EEEE3B1D8}</c15:txfldGUID>
                       <c15:f>calcs!$T$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6607,7 +6610,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5160F406-2704-40AC-BB1D-481721E9CA0E}</c15:txfldGUID>
+                      <c15:txfldGUID>{6042171F-F494-4AE0-84FF-201F6D6D5DB7}</c15:txfldGUID>
                       <c15:f>calcs!$U$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6648,7 +6651,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{F2FF2350-C333-414F-A1E6-7A04CF56EF8A}</c15:txfldGUID>
+                      <c15:txfldGUID>{C03256AC-BA83-4C8E-BAC8-DCFA9198873C}</c15:txfldGUID>
                       <c15:f>calcs!$V$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6689,7 +6692,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{88611894-D76C-4647-9617-ABA60AFB4BEA}</c15:txfldGUID>
+                      <c15:txfldGUID>{04D92674-82A7-4408-BFC1-68739034B17A}</c15:txfldGUID>
                       <c15:f>calcs!$W$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6730,7 +6733,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{47657DF3-FC9B-40D2-BB35-A3E28A96D17D}</c15:txfldGUID>
+                      <c15:txfldGUID>{D1230F48-6512-4F89-B8E9-28C5A13CA4F9}</c15:txfldGUID>
                       <c15:f>calcs!$X$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6771,7 +6774,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{52B68A95-0F7D-4E92-AC23-C253495D1B0A}</c15:txfldGUID>
+                      <c15:txfldGUID>{4E12AF0F-0D0B-47BB-9CDB-6A1C00D90FDE}</c15:txfldGUID>
                       <c15:f>calcs!$Y$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6812,7 +6815,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{EC35CF58-29A0-4B70-8996-746588ED1A67}</c15:txfldGUID>
+                      <c15:txfldGUID>{2D67A013-77E9-43E9-90D1-19EF6A389879}</c15:txfldGUID>
                       <c15:f>calcs!$Z$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6853,7 +6856,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{3D63415A-2314-4DCB-98DB-CC33BEF0D329}</c15:txfldGUID>
+                      <c15:txfldGUID>{B40432EE-35D1-4CDA-8CB6-CAAD3022A67D}</c15:txfldGUID>
                       <c15:f>calcs!$AA$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6894,7 +6897,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{A6589455-1124-40A3-8051-DB318BBA9263}</c15:txfldGUID>
+                      <c15:txfldGUID>{EB840C98-F01C-4969-A553-21B1526E6092}</c15:txfldGUID>
                       <c15:f>calcs!$AB$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6935,7 +6938,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{2C5A96F3-1ED3-48D6-9E7F-F63EFB495E0A}</c15:txfldGUID>
+                      <c15:txfldGUID>{7DEBE99F-D53E-4998-9E38-0015FF2529B4}</c15:txfldGUID>
                       <c15:f>calcs!$AC$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -6976,7 +6979,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{CE072F2A-C688-4688-87E0-20AFBDA2A93C}</c15:txfldGUID>
+                      <c15:txfldGUID>{2D1ECED0-68E7-4F75-AAC1-77F4861D917D}</c15:txfldGUID>
                       <c15:f>calcs!$AD$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -7017,7 +7020,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4DE14F4B-7D65-4FC1-975A-BDD056234996}</c15:txfldGUID>
+                      <c15:txfldGUID>{E683EA6D-20E0-4A85-B1EC-0B8366D760B2}</c15:txfldGUID>
                       <c15:f>calcs!$AE$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -7058,7 +7061,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{D619C517-DAFC-43CD-B0E2-249F7E14DBBD}</c15:txfldGUID>
+                      <c15:txfldGUID>{5DD9D42F-8F20-4BAD-A57C-D04CE5E5A26D}</c15:txfldGUID>
                       <c15:f>calcs!$AF$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -7099,7 +7102,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{4B1812C2-D419-40AD-9C59-79DDFD2B87D5}</c15:txfldGUID>
+                      <c15:txfldGUID>{A14925E9-CEDC-4F5F-B21E-91B924257B04}</c15:txfldGUID>
                       <c15:f>calcs!$AG$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -7140,7 +7143,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{5394315F-FA09-4AB6-98C6-F23522E72F64}</c15:txfldGUID>
+                      <c15:txfldGUID>{4209D686-BB72-41AF-A8D6-34EF921251AD}</c15:txfldGUID>
                       <c15:f>calcs!$AH$70</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -7719,8 +7722,8 @@
         <a:xfrm>
           <a:off x="325877" y="4038600"/>
           <a:ext cx="8988869" cy="228436"/>
-          <a:chOff x="306828" y="4108026"/>
-          <a:chExt cx="8729080" cy="223568"/>
+          <a:chOff x="306828" y="4108028"/>
+          <a:chExt cx="8729080" cy="223566"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
@@ -7794,7 +7797,7 @@
             </xdr:nvSpPr>
             <xdr:spPr bwMode="auto">
               <a:xfrm>
-                <a:off x="306828" y="4108026"/>
+                <a:off x="306828" y="4108028"/>
                 <a:ext cx="8729080" cy="163196"/>
               </a:xfrm>
               <a:prstGeom prst="rect">
@@ -8078,8 +8081,8 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8096,22 +8099,22 @@
     <row r="1" spans="1:7" s="4" customFormat="1" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" ht="315.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:7" s="7" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="8" t="s">
@@ -8251,7 +8254,7 @@
         <v>43760</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -8271,7 +8274,7 @@
         <v>43778</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -8291,7 +8294,7 @@
         <v>43772</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -8299,14 +8302,17 @@
         <f>ROW(B13)-calcs!$D$5</f>
         <v>-2</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>37</v>
+      <c r="C13" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="D13" s="1">
         <v>43786</v>
       </c>
       <c r="E13" s="1">
         <v>43786</v>
+      </c>
+      <c r="F13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -8314,7 +8320,7 @@
         <f>ROW(B14)-calcs!$D$5</f>
         <v>-1</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="11" t="s">
         <v>31</v>
       </c>
       <c r="D14" s="5">
@@ -8324,6 +8330,9 @@
       <c r="E14" s="5">
         <f>Activities[[#This Row],[START]]+7</f>
         <v>43789</v>
+      </c>
+      <c r="F14" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -8331,7 +8340,7 @@
         <f>ROW(B15)-calcs!$D$5</f>
         <v>0</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="11" t="s">
         <v>32</v>
       </c>
       <c r="D15" s="5">
@@ -8341,6 +8350,9 @@
       <c r="E15" s="5">
         <f>Activities[[#This Row],[START]]+6</f>
         <v>43793</v>
+      </c>
+      <c r="F15" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -8348,7 +8360,7 @@
         <f>ROW(B16)-calcs!$D$5</f>
         <v>1</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>33</v>
       </c>
       <c r="D16" s="5">
@@ -8358,14 +8370,17 @@
         <f>Activities[[#This Row],[START]]+8</f>
         <v>43797</v>
       </c>
+      <c r="F16" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="17" spans="2:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>ROW(B17)-calcs!$D$5</f>
         <v>2</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>34</v>
+      <c r="C17" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="D17" s="5">
         <f>D16+2</f>
@@ -8374,25 +8389,28 @@
       <c r="E17" s="5">
         <v>43804</v>
       </c>
+      <c r="F17" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="18" spans="2:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18">
         <f>ROW(B18)-calcs!$D$5</f>
         <v>3</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="11" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="1">
         <v>43804</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19">
         <f>ROW(B19)-calcs!$D$5</f>
         <v>4</v>
       </c>
-      <c r="C19" s="13"/>
+      <c r="C19" s="11"/>
       <c r="D19" s="1"/>
     </row>
   </sheetData>
@@ -8481,7 +8499,7 @@
       </c>
       <c r="D3" s="1">
         <f ca="1">TODAY()</f>
-        <v>43785</v>
+        <v>43801</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -12899,23 +12917,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9677210f24a1be23c92c90fd886aa0aa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="60e05723c5c1908df1a1a4ebf11d344e" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -13126,25 +13127,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED11D93F-21D3-4821-9768-A0F99C41A8EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{983CAFE3-5C64-4732-BD1D-A9D00643597D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5BB6EA-B4A9-4FD0-A581-32FE787E0D00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13161,4 +13161,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{983CAFE3-5C64-4732-BD1D-A9D00643597D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED11D93F-21D3-4821-9768-A0F99C41A8EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>